<commit_message>
updated ui and fields in roster data
</commit_message>
<xml_diff>
--- a/dummy-roster.xlsx
+++ b/dummy-roster.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shivam\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shivam\Downloads\ManageCX-zip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB18C40-43A3-4998-8C27-363FC2AA8F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06511946-12D5-4BD0-9B23-4A819ACF4966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{87CBA0D9-03C4-4FBE-A6D0-40AD188BADB2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
   <si>
     <t>Monday</t>
   </si>
@@ -66,37 +66,28 @@
     <t>Emp Id</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>TL Name</t>
-  </si>
-  <si>
-    <t>Emp A</t>
-  </si>
-  <si>
-    <t>Emp B</t>
-  </si>
-  <si>
-    <t>Emp C</t>
-  </si>
-  <si>
-    <t>Emp D</t>
-  </si>
-  <si>
-    <t>Emp E</t>
-  </si>
-  <si>
-    <t>Emp F</t>
-  </si>
-  <si>
-    <t>Emp G</t>
-  </si>
-  <si>
     <t>Leave</t>
   </si>
   <si>
     <t>WO</t>
+  </si>
+  <si>
+    <t>Transport Status</t>
+  </si>
+  <si>
+    <t>Work Status</t>
+  </si>
+  <si>
+    <t>Company Transport</t>
+  </si>
+  <si>
+    <t>Self Transport</t>
+  </si>
+  <si>
+    <t>WFO</t>
+  </si>
+  <si>
+    <t>WFH</t>
   </si>
 </sst>
 </file>
@@ -134,13 +125,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,7 +449,7 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E2"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -467,74 +458,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="I1" s="2"/>
+      <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1" t="s">
+      <c r="K1" s="2"/>
+      <c r="L1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1" t="s">
+      <c r="M1" s="2"/>
+      <c r="N1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1" t="s">
+      <c r="O1" s="2"/>
+      <c r="P1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="1"/>
+      <c r="Q1" s="2"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <v>45803</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="2">
+      <c r="E2" s="2"/>
+      <c r="F2" s="3">
         <v>45804</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="2">
+      <c r="G2" s="2"/>
+      <c r="H2" s="3">
         <v>45805</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="2">
+      <c r="I2" s="2"/>
+      <c r="J2" s="3">
         <v>45806</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="2">
+      <c r="K2" s="2"/>
+      <c r="L2" s="3">
         <v>45807</v>
       </c>
-      <c r="M2" s="1"/>
-      <c r="N2" s="2">
+      <c r="M2" s="2"/>
+      <c r="N2" s="3">
         <v>45808</v>
       </c>
-      <c r="O2" s="1"/>
-      <c r="P2" s="2">
+      <c r="O2" s="2"/>
+      <c r="P2" s="3">
         <v>45809</v>
       </c>
-      <c r="Q2" s="2"/>
+      <c r="Q2" s="3"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -584,42 +575,45 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.625</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="G4" s="3">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G4" s="1">
         <v>0.625</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="J4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="M4" s="3">
-        <v>0.625</v>
-      </c>
-      <c r="N4" s="3">
+        <v>11</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="N4" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O4" s="1">
         <v>0.75</v>
       </c>
-      <c r="P4" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="Q4" s="3">
+      <c r="P4" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="Q4" s="1">
         <v>0.625</v>
       </c>
     </row>
@@ -628,42 +622,45 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="3">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1">
         <v>0.29166666666666669</v>
       </c>
-      <c r="E5" s="3">
-        <v>0.625</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="E5" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G5" s="1">
         <v>0.625</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="J5" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" s="3">
+        <v>11</v>
+      </c>
+      <c r="L5" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="M5" s="3">
-        <v>0.625</v>
-      </c>
-      <c r="N5" s="3">
+      <c r="M5" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="N5" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5" s="1">
         <v>0.75</v>
       </c>
-      <c r="P5" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="Q5" s="3">
+      <c r="P5" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="Q5" s="1">
         <v>0.625</v>
       </c>
     </row>
@@ -674,41 +671,44 @@
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="3">
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="F6" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0.625</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="I6" s="3">
+      <c r="F6" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="I6" s="1">
         <v>0.625</v>
       </c>
       <c r="J6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="M6" s="3">
+        <v>11</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="M6" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6" s="1">
         <v>0.75</v>
       </c>
       <c r="P6" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
@@ -716,42 +716,45 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1">
         <v>0.375</v>
       </c>
-      <c r="E7" s="3">
-        <v>0.625</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="G7" s="3">
+      <c r="E7" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G7" s="1">
         <v>0.625</v>
       </c>
       <c r="H7" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="J7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L7" s="3">
+        <v>11</v>
+      </c>
+      <c r="L7" s="1">
         <v>0.125</v>
       </c>
-      <c r="M7" s="3">
-        <v>0.625</v>
-      </c>
-      <c r="N7" s="3">
+      <c r="M7" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="N7" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="O7" s="3">
+      <c r="O7" s="1">
         <v>0.75</v>
       </c>
-      <c r="P7" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="Q7" s="3">
+      <c r="P7" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="Q7" s="1">
         <v>0.625</v>
       </c>
     </row>
@@ -760,42 +763,45 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="3">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <v>0.54166666666666663</v>
       </c>
-      <c r="F8" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="G8" s="3">
+      <c r="F8" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G8" s="1">
         <v>0.625</v>
       </c>
       <c r="H8" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="J8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L8" s="3">
+        <v>11</v>
+      </c>
+      <c r="L8" s="1">
         <v>0.375</v>
       </c>
-      <c r="M8" s="3">
+      <c r="M8" s="1">
         <v>0.54166666666666663</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8" s="1">
         <v>0.75</v>
       </c>
-      <c r="P8" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="Q8" s="3">
+      <c r="P8" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="Q8" s="1">
         <v>0.625</v>
       </c>
     </row>
@@ -804,45 +810,48 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="3">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1">
         <v>0.375</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="1">
         <v>0.66666666666666663</v>
       </c>
-      <c r="F9" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="G9" s="3">
+      <c r="F9" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G9" s="1">
         <v>0.625</v>
       </c>
       <c r="H9" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="K9" s="3">
-        <v>0.625</v>
-      </c>
-      <c r="L9" s="3">
+        <v>10</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="L9" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9" s="1">
         <v>0.66666666666666663</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O9" s="1">
         <v>0.75</v>
       </c>
-      <c r="P9" s="3">
+      <c r="P9" s="1">
         <v>0.375</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="Q9" s="1">
         <v>0.625</v>
       </c>
     </row>
@@ -851,40 +860,43 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="3">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="E10" s="3">
-        <v>0.625</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="G10" s="3">
+      <c r="E10" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G10" s="1">
         <v>0.625</v>
       </c>
       <c r="H10" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="J10" t="s">
-        <v>20</v>
-      </c>
-      <c r="L10" s="3">
+        <v>11</v>
+      </c>
+      <c r="L10" s="1">
         <v>0.45833333333333331</v>
       </c>
-      <c r="M10" s="3">
-        <v>0.625</v>
-      </c>
-      <c r="N10" s="3">
+      <c r="M10" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="N10" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="O10" s="3">
+      <c r="O10" s="1">
         <v>0.75</v>
       </c>
       <c r="P10" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>